<commit_message>
add mixed precision and XLA compilation
</commit_message>
<xml_diff>
--- a/training_speed_mirrored_strategy.xlsx
+++ b/training_speed_mirrored_strategy.xlsx
@@ -20,24 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Average GPU utilization</t>
+  </si>
   <si>
     <t xml:space="preserve">batch_size = 256</t>
   </si>
   <si>
-    <t xml:space="preserve">Average GPU utilization</t>
-  </si>
-  <si>
     <t xml:space="preserve">GPU/epochs</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; 30 %%</t>
-  </si>
-  <si>
     <t xml:space="preserve">batch_size = 128</t>
   </si>
   <si>
-    <t xml:space="preserve">batch_size = 64</t>
+    <t xml:space="preserve">batch_size = 2048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size = 4096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low recall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size = 1024</t>
   </si>
 </sst>
 </file>
@@ -133,10 +139,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G21"/>
+  <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4:G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -148,11 +154,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.82"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -169,9 +177,6 @@
       <c r="E3" s="0" t="n">
         <v>256</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
@@ -180,16 +185,34 @@
       <c r="C4" s="0" t="n">
         <v>113.73</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>215.72</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>418.85</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>101.97</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>194.36</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>376.06</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E6" s="0" t="n">
+        <v>355.88</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
@@ -198,7 +221,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,13 +260,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="C17" s="0" t="n">
         <v>64</v>
       </c>
@@ -258,6 +278,12 @@
       <c r="B18" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>55.06</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>97.29</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
@@ -268,9 +294,99 @@
       <c r="B20" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>56.11</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>104.92</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>52.25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>54.36</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>112.19</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix mixed precision policy
</commit_message>
<xml_diff>
--- a/training_speed_mirrored_strategy.xlsx
+++ b/training_speed_mirrored_strategy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Average GPU utilization</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">batch_size = 1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1024, mixed precision, XLA</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -73,6 +76,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,8 +126,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,6 +144,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -139,10 +212,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:G35"/>
+  <dimension ref="B1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G16" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -151,11 +224,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -310,7 +384,7 @@
       <c r="B23" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -355,6 +429,9 @@
       <c r="B30" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="G30" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="n">
@@ -366,6 +443,15 @@
       <c r="E31" s="0" t="n">
         <v>256</v>
       </c>
+      <c r="H31" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="n">
@@ -374,11 +460,20 @@
       <c r="D32" s="0" t="n">
         <v>112.19</v>
       </c>
+      <c r="G32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>123.31</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G33" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="n">
@@ -387,9 +482,18 @@
       <c r="D34" s="0" t="n">
         <v>116.69</v>
       </c>
+      <c r="G34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>112.78</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add one more layer
</commit_message>
<xml_diff>
--- a/training_speed_mirrored_strategy.xlsx
+++ b/training_speed_mirrored_strategy.xlsx
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +83,7 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -214,18 +216,18 @@
   </sheetPr>
   <dimension ref="B1:J35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G16" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>